<commit_message>
Tudo funcionando na interface!!!
</commit_message>
<xml_diff>
--- a/interface/appInterface/telaPrimaria/promocoes.xlsx
+++ b/interface/appInterface/telaPrimaria/promocoes.xlsx
@@ -767,27 +767,27 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="0" t="inlineStr">
         <is>
           <t>Mundo Animal</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" s="0" t="inlineStr">
         <is>
           <t>Torres de batata</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C16" s="0" t="inlineStr">
         <is>
           <t>30%</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D16" s="0" t="inlineStr">
         <is>
           <t>-29.709187307987996</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="E16" s="0" t="inlineStr">
         <is>
           <t>-52.42625533514549</t>
         </is>

</xml_diff>